<commit_message>
Info folder updated with binance and docker support
</commit_message>
<xml_diff>
--- a/src/Info/Exchange_Price_service.xlsx
+++ b/src/Info/Exchange_Price_service.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A-7985\Downloads\exchange-price-service\src\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26951FE9-9C41-4240-8762-6340AF5A3429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE717F3F-38DE-41A5-B9D6-52C6DB3C8AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -747,15 +747,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>13</xdr:col>
-          <xdr:colOff>266700</xdr:colOff>
+          <xdr:colOff>175260</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>137160</xdr:rowOff>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>14</xdr:col>
-          <xdr:colOff>160020</xdr:colOff>
+          <xdr:colOff>68580</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>106680</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1154,16 +1154,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>18</xdr:col>
-          <xdr:colOff>350520</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
+          <xdr:col>17</xdr:col>
+          <xdr:colOff>571500</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>129540</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>19</xdr:col>
-          <xdr:colOff>327660</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>83820</xdr:rowOff>
+          <xdr:col>18</xdr:col>
+          <xdr:colOff>548640</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>99060</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1609,7 +1609,7 @@
   <dimension ref="N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1682,15 +1682,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>13</xdr:col>
-                <xdr:colOff>266700</xdr:colOff>
+                <xdr:colOff>175260</xdr:colOff>
                 <xdr:row>5</xdr:row>
-                <xdr:rowOff>137160</xdr:rowOff>
+                <xdr:rowOff>175260</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>14</xdr:col>
-                <xdr:colOff>160020</xdr:colOff>
+                <xdr:colOff>68580</xdr:colOff>
                 <xdr:row>8</xdr:row>
-                <xdr:rowOff>106680</xdr:rowOff>
+                <xdr:rowOff>144780</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1831,16 +1831,16 @@
           <objectPr defaultSize="0" r:id="rId21">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>18</xdr:col>
-                <xdr:colOff>350520</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>17</xdr:col>
+                <xdr:colOff>571500</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>129540</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>19</xdr:col>
-                <xdr:colOff>327660</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>83820</xdr:rowOff>
+                <xdr:col>18</xdr:col>
+                <xdr:colOff>548640</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>99060</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>

</xml_diff>

<commit_message>
price subscription sample is ready
</commit_message>
<xml_diff>
--- a/src/Info/Exchange_Price_service.xlsx
+++ b/src/Info/Exchange_Price_service.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A-7985\Downloads\exchange-price-service\src\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE717F3F-38DE-41A5-B9D6-52C6DB3C8AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87A97D0-4A78-4E78-8779-558E5236E659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project structure and basic cod" sheetId="1" r:id="rId1"/>
     <sheet name="Docker Price Services" sheetId="2" r:id="rId2"/>
+    <sheet name="Binance Streamer" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -223,7 +224,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{807DA955-3CA3-700E-FDB9-05E3C64C343C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -267,7 +268,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2FCE8C6-DD27-A46D-3142-2770AA0AFC0F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -311,7 +312,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FECE7E94-61D2-8A4C-A2DE-FBF18B323CE2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -355,7 +356,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EFE8D10-2572-D713-B5AE-A5C9EC729A5C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -399,7 +400,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A12A3005-04DC-86CE-8B6C-81AE2FAFEDDC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -443,7 +444,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3942FBBE-43A1-2767-CA83-4C5E7EBA69D0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -492,7 +493,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F1EBF9B-5347-61BC-5AB0-B46CE593D24E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -536,7 +537,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98860557-2316-F085-C45F-B11002C8884F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -580,7 +581,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5950FE0-CE97-1F89-8BE6-5BC071E6EF32}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -629,7 +630,7 @@
                   <a14:compatExt spid="_x0000_s2049"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{249FC9FA-8181-FE23-874C-2EF4F45EE832}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -650,23 +651,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -697,7 +685,7 @@
                   <a14:compatExt spid="_x0000_s2050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{969FBCBD-338D-E9F7-6147-0D4D3CCF8D92}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -718,23 +706,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -765,7 +740,7 @@
                   <a14:compatExt spid="_x0000_s2051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E76AAEA-1BB1-304C-8629-B532D6486F20}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -786,23 +761,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -833,7 +795,7 @@
                   <a14:compatExt spid="_x0000_s2052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{125A4CD0-909B-81FC-D023-C749DCF7DA98}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -854,23 +816,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -901,7 +850,7 @@
                   <a14:compatExt spid="_x0000_s2053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AC3C381-FD26-FB40-FE09-5679E98A2099}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -922,23 +871,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -969,7 +905,7 @@
                   <a14:compatExt spid="_x0000_s2054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76937141-5984-64F4-15FF-C6B6150757BB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -990,23 +926,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1037,7 +960,7 @@
                   <a14:compatExt spid="_x0000_s2055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE024367-F8B8-B931-4721-C4CEAF0864D9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1058,23 +981,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1105,7 +1015,7 @@
                   <a14:compatExt spid="_x0000_s2056"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CE15DF7-9928-CA9F-9E0F-46374000498B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1126,23 +1036,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1173,7 +1070,7 @@
                   <a14:compatExt spid="_x0000_s2057"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27D534C1-CFCD-347F-73EC-9157FD678C16}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1194,23 +1091,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1218,6 +1102,99 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>544192</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>88510</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AA10ACC-FAB1-BBB4-7627-B599E488CFB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="731520"/>
+          <a:ext cx="9078592" cy="6306430"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>600635</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>17929</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>249437</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>37122</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61704B1C-F52A-856B-A414-1D3768FDF586}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6087035" y="914400"/>
+          <a:ext cx="8792802" cy="5039428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1486,7 +1463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:Q129"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="H117" sqref="H117"/>
     </sheetView>
   </sheetViews>
@@ -1608,7 +1585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A40CA0-CBFA-4B49-965C-46DAACF5C8EF}">
   <dimension ref="N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -1852,4 +1829,19 @@
     </mc:AlternateContent>
   </oleObjects>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D325E0-77E4-4527-9758-17B4270AA354}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>